<commit_message>
Novas Tabelas mapeadas LN
</commit_message>
<xml_diff>
--- a/Documentação/Tabelas_LN/tccom125-Ctas bancarias por parceiro neg credor.xlsx
+++ b/Documentação/Tabelas_LN/tccom125-Ctas bancarias por parceiro neg credor.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="525" windowWidth="19815" windowHeight="7110"/>
@@ -14,7 +14,7 @@
     <definedName name="ttadv.type">enums!$D$3:$D$16</definedName>
     <definedName name="ttyeno">enums!$B$3:$B$4</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -34,8 +34,9 @@
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
-          <t>name: ttadv420._compnr
-type: integer
+          <t>name: ttadv420.cpac
+type: string
+primaryKey: true
 headerSession: ttadv4520m100</t>
         </r>
       </text>
@@ -50,7 +51,7 @@
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
-          <t>name: ttadv420.cpac
+          <t>name: ttadv420.cmod
 type: string
 primaryKey: true
 headerSession: ttadv4520m100</t>
@@ -67,7 +68,7 @@
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
-          <t>name: ttadv420.cmod
+          <t>name: ttadv420.flno
 type: string
 primaryKey: true
 headerSession: ttadv4520m100</t>
@@ -84,30 +85,13 @@
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
-          <t>name: ttadv420.flno
-type: string
-primaryKey: true
-headerSession: ttadv4520m100</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
           <t>name: table.desc
 type: string
 headerSession: ttadv4520m100</t>
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -124,7 +108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -141,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -158,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -175,7 +159,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -191,7 +175,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -207,7 +191,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -224,7 +208,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -241,7 +225,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -257,7 +241,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -273,7 +257,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -290,7 +274,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0">
+    <comment ref="P1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -306,7 +290,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0">
+    <comment ref="Q1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -322,7 +306,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0">
+    <comment ref="R1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -343,7 +327,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="74">
   <si>
     <t/>
   </si>
@@ -570,8 +554,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -581,15 +565,24 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="9"/>
       <color indexed="60"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="9"/>
       <color indexed="9"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -622,14 +615,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -719,7 +713,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -754,7 +747,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -930,688 +922,656 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:18">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4">
+        <v>1</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="4">
+        <v>9</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0</v>
+      </c>
+      <c r="J3" s="4">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="K3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" s="4">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0</v>
+      </c>
+      <c r="J4" s="4">
+        <v>3</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" s="4">
+        <v>34</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4">
+        <v>4</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P5" s="4">
+        <v>34</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0</v>
+      </c>
+      <c r="J6" s="4">
+        <v>5</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P6" s="4">
+        <v>15</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0</v>
+      </c>
+      <c r="J7" s="4">
+        <v>6</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P7" s="4">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4">
+        <v>7</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P8" s="4">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="Q8" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="E9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="G9" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="H9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="M2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="I9" s="4">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4">
+        <v>8</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="O2" t="s">
-        <v>40</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="B10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0</v>
+      </c>
+      <c r="J10" s="4">
+        <v>200</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="O10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="Q2">
-        <v>9</v>
-      </c>
-      <c r="R2" t="s">
-        <v>41</v>
-      </c>
-      <c r="S2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="P10" s="4">
+        <v>34</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="B11" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="C11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="4" t="s">
+      <c r="E11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="G11" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="H11" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
+      <c r="I11" s="4">
+        <v>0</v>
+      </c>
+      <c r="J11" s="4">
+        <v>201</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P11" s="4">
         <v>2</v>
       </c>
-      <c r="L3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="M3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N3" t="s">
-        <v>32</v>
-      </c>
-      <c r="O3" t="s">
-        <v>43</v>
-      </c>
-      <c r="P3" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q3">
-        <v>3</v>
-      </c>
-      <c r="R3" t="s">
-        <v>44</v>
-      </c>
-      <c r="S3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>3</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="M4" t="s">
-        <v>8</v>
-      </c>
-      <c r="N4" t="s">
-        <v>32</v>
-      </c>
-      <c r="O4" t="s">
-        <v>46</v>
-      </c>
-      <c r="P4" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q4">
-        <v>34</v>
-      </c>
-      <c r="R4" t="s">
-        <v>47</v>
-      </c>
-      <c r="S4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>4</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="M5" t="s">
-        <v>8</v>
-      </c>
-      <c r="N5" t="s">
-        <v>32</v>
-      </c>
-      <c r="O5" t="s">
-        <v>50</v>
-      </c>
-      <c r="P5" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q5">
-        <v>34</v>
-      </c>
-      <c r="R5" t="s">
-        <v>51</v>
-      </c>
-      <c r="S5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>5</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="M6" t="s">
-        <v>8</v>
-      </c>
-      <c r="N6" t="s">
-        <v>32</v>
-      </c>
-      <c r="O6" t="s">
-        <v>54</v>
-      </c>
-      <c r="P6" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q6">
-        <v>15</v>
-      </c>
-      <c r="R6" t="s">
-        <v>55</v>
-      </c>
-      <c r="S6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>6</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="M7" t="s">
-        <v>8</v>
-      </c>
-      <c r="N7" t="s">
-        <v>32</v>
-      </c>
-      <c r="O7" t="s">
-        <v>58</v>
-      </c>
-      <c r="P7" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q7">
-        <v>35</v>
-      </c>
-      <c r="R7" t="s">
-        <v>59</v>
-      </c>
-      <c r="S7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>7</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="M8" t="s">
-        <v>8</v>
-      </c>
-      <c r="N8" t="s">
-        <v>32</v>
-      </c>
-      <c r="O8" t="s">
-        <v>62</v>
-      </c>
-      <c r="P8" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q8">
-        <v>12</v>
-      </c>
-      <c r="R8" t="s">
-        <v>63</v>
-      </c>
-      <c r="S8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>0</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>8</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="M9" t="s">
-        <v>7</v>
-      </c>
-      <c r="N9" t="s">
-        <v>0</v>
-      </c>
-      <c r="O9" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9" t="s">
-        <v>0</v>
-      </c>
-      <c r="S9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>200</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="M10" t="s">
-        <v>8</v>
-      </c>
-      <c r="N10" t="s">
-        <v>32</v>
-      </c>
-      <c r="O10" t="s">
-        <v>46</v>
-      </c>
-      <c r="P10" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q10">
-        <v>34</v>
-      </c>
-      <c r="R10" t="s">
-        <v>67</v>
-      </c>
-      <c r="S10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>0</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>201</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="M11" t="s">
-        <v>8</v>
-      </c>
-      <c r="N11" t="s">
-        <v>70</v>
-      </c>
-      <c r="O11" t="s">
-        <v>71</v>
-      </c>
-      <c r="P11" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q11">
-        <v>2</v>
-      </c>
-      <c r="R11" t="s">
+      <c r="Q11" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="S11" t="s">
+      <c r="R11" s="4" t="s">
         <v>73</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M1048575 F2:F1048575">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048575 E2:E1048575">
       <formula1>ttyeno</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P1048575">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O1048575">
       <formula1>ttadv.type</formula1>
     </dataValidation>
   </dataValidations>
@@ -1621,14 +1581,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1636,7 +1596,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1650,7 +1610,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1664,7 +1624,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1678,7 +1638,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="C5">
         <v>3</v>
       </c>
@@ -1686,7 +1646,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="C6">
         <v>4</v>
       </c>
@@ -1694,7 +1654,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="C7">
         <v>5</v>
       </c>
@@ -1702,7 +1662,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="C8">
         <v>6</v>
       </c>
@@ -1710,7 +1670,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="C9">
         <v>7</v>
       </c>
@@ -1718,7 +1678,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="C10">
         <v>8</v>
       </c>
@@ -1726,7 +1686,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="C11">
         <v>9</v>
       </c>
@@ -1734,7 +1694,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="C12">
         <v>10</v>
       </c>
@@ -1742,7 +1702,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="C13">
         <v>11</v>
       </c>
@@ -1750,7 +1710,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="C14">
         <v>12</v>
       </c>
@@ -1758,7 +1718,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="C15">
         <v>13</v>
       </c>
@@ -1766,7 +1726,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="C16">
         <v>14</v>
       </c>

</xml_diff>